<commit_message>
added active and retirement stacked bar charts
</commit_message>
<xml_diff>
--- a/mil_pay.xlsx
+++ b/mil_pay.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dollahite/Recreational Coding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dollahite/Recreational Coding/MilitaryCivilianPayComparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4440DE07-5EDE-934C-B79A-AD5FE5F8163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612712F3-7ADC-E948-B126-345A058E90E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{8D5A86E9-A945-2546-8546-5034BE9E28AD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{8D5A86E9-A945-2546-8546-5034BE9E28AD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ActiveRetire" sheetId="1" r:id="rId1"/>
+    <sheet name="ReserveRetire" sheetId="2" r:id="rId2"/>
+    <sheet name="Separate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>Calendar Year</t>
   </si>
@@ -167,10 +169,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,23 +489,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DA569B-4D87-EC48-BC2D-6A424EA30996}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J62" sqref="A1:J62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="17.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1802,4 +1803,1271 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AA25B2-E66F-B744-B8F1-8E1F382A56E6}">
+  <dimension ref="A1:J62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
+        <v>7274</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6">
+        <v>364</v>
+      </c>
+      <c r="F2" s="6">
+        <v>73</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>52730</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6">
+        <v>2637</v>
+      </c>
+      <c r="F3" s="6">
+        <v>542</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6">
+        <v>63066</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6">
+        <v>2714</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2523</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2026</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6">
+        <v>73746</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6">
+        <v>2950</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4000</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>2027</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6">
+        <v>77638</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6">
+        <v>3106</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4327</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>2028</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6">
+        <v>80122</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
+        <v>3205</v>
+      </c>
+      <c r="F7" s="6">
+        <v>4588</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>2029</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6">
+        <v>81364</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6">
+        <v>3255</v>
+      </c>
+      <c r="F8" s="6">
+        <v>4787</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>2030</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <v>84085</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6">
+        <v>3363</v>
+      </c>
+      <c r="F9" s="6">
+        <v>5083</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>2031</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6">
+        <v>85446</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6">
+        <v>3418</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5308</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>2032</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6">
+        <v>38595</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6">
+        <v>1544</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2463</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>2033</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6">
+        <v>16430</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6">
+        <v>657</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1078</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>2034</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6">
+        <v>17626</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4333</v>
+      </c>
+      <c r="E13" s="6">
+        <v>705</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1188</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>2035</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>17909</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6">
+        <v>716</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1240</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>2036</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6">
+        <v>18302</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6">
+        <v>732</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1302</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>2037</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6">
+        <v>18499</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6">
+        <v>740</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1352</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2038</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6">
+        <v>18725</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6">
+        <v>749</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1406</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>2039</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="6">
+        <v>20034</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6">
+        <v>801</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1546</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>2040</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6">
+        <v>21020</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6">
+        <v>841</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1667</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>2041</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="6">
+        <v>21215</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6">
+        <v>849</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1729</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>2042</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6">
+        <v>7072</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6">
+        <v>283</v>
+      </c>
+      <c r="F21" s="6">
+        <v>592</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>2043</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>2044</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>2045</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>2046</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>2047</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>2048</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>2049</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>2050</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>2051</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>2052</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>2053</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>2054</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>2055</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>2056</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>2057</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>2058</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="6">
+        <v>21337</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="6">
+        <v>21337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>2059</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="6">
+        <v>32006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>2060</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="6">
+        <v>32006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>2061</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="6">
+        <v>32006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>2062</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="6">
+        <v>32006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>2063</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="6">
+        <v>32006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>2064</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="6">
+        <v>32006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>2065</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H44" s="6">
+        <v>7173</v>
+      </c>
+      <c r="I44" s="6">
+        <v>6474</v>
+      </c>
+      <c r="J44" s="6">
+        <v>45653</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>2066</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H45" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I45" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J45" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>2067</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H46" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I46" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J46" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>2068</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H47" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I47" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J47" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>2069</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H48" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I48" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J48" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H49" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I49" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J49" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>2071</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H50" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I50" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J50" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>2072</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H51" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I51" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J51" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>2073</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H52" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I52" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J52" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>2074</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H53" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I53" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J53" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>2075</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H54" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I54" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J54" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>2076</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H55" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I55" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J55" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>2077</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H56" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I56" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J56" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>2078</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H57" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I57" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J57" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>2079</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H58" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I58" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J58" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H59" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I59" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J59" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>2081</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H60" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I60" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J60" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>2082</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="6">
+        <v>32006</v>
+      </c>
+      <c r="H61" s="6">
+        <v>10760</v>
+      </c>
+      <c r="I61" s="6">
+        <v>9711</v>
+      </c>
+      <c r="J61" s="6">
+        <v>52477</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>2083</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="6">
+        <v>13336</v>
+      </c>
+      <c r="H62" s="6">
+        <v>4483</v>
+      </c>
+      <c r="I62" s="6">
+        <v>4046</v>
+      </c>
+      <c r="J62" s="6">
+        <v>21865</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F7DF07-F919-494F-8795-A8B288B06747}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>